<commit_message>
CSS.pptx & asistencia 2005
</commit_message>
<xml_diff>
--- a/asistencia/Paralelo 1.xlsx
+++ b/asistencia/Paralelo 1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>15-may</t>
+  </si>
+  <si>
+    <t>20-may</t>
   </si>
 </sst>
 </file>
@@ -269,13 +272,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0">
-  <autoFilter ref="A1:D31"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0">
+  <autoFilter ref="A1:E31"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="MATRICULA"/>
     <tableColumn id="2" name="NOMBRE_ESTUDIANTE"/>
     <tableColumn id="3" name="13-may"/>
     <tableColumn id="4" name="15-may"/>
+    <tableColumn id="5" name="20-may"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -566,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -578,7 +582,7 @@
     <col min="2" max="2" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +595,11 @@
       <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -605,8 +612,11 @@
       <c r="D2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -614,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -627,8 +637,11 @@
       <c r="D4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -636,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -649,8 +662,11 @@
       <c r="D6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -663,8 +679,11 @@
       <c r="D7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -677,8 +696,11 @@
       <c r="D8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -691,8 +713,11 @@
       <c r="D9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -705,8 +730,11 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -719,8 +747,11 @@
       <c r="D11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -733,8 +764,11 @@
       <c r="D12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -747,8 +781,11 @@
       <c r="D13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -761,8 +798,11 @@
       <c r="D14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -775,8 +815,11 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -789,8 +832,11 @@
       <c r="D16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -803,8 +849,11 @@
       <c r="D17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -817,8 +866,11 @@
       <c r="D18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -831,16 +883,22 @@
       <c r="D19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -853,8 +911,11 @@
       <c r="D21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -867,8 +928,11 @@
       <c r="D22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -881,8 +945,11 @@
       <c r="D23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -895,8 +962,11 @@
       <c r="D24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -909,8 +979,11 @@
       <c r="D25" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -923,8 +996,11 @@
       <c r="D26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -937,8 +1013,11 @@
       <c r="D27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -951,8 +1030,11 @@
       <c r="D28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -965,8 +1047,11 @@
       <c r="D29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -979,8 +1064,11 @@
       <c r="D30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -991,6 +1079,9 @@
         <v>62</v>
       </c>
       <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>